<commit_message>
Implement logging, Add AccountsMapperTest
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PrasadKarunagoda\github2\finance-tracker-server\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEDD8E1-D106-4C9D-815F-AC6B81B5BE8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125504E3-E3CB-465B-AD54-6783CE96DBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{098832E3-9C45-44C4-8C94-60A0EB67C861}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{098832E3-9C45-44C4-8C94-60A0EB67C861}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -415,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692EEC09-387A-43B1-8C30-02B194D7C147}">
   <dimension ref="D3:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -455,4 +456,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3742BC-9C90-4905-8931-84C893A18ECC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>